<commit_message>
Update remote Docker deployment guide with new structure
- Updated deployment guide to reflect new organized file structure
- Added comprehensive server setup instructions
- Included all available Docker services and their usage
- Added troubleshooting section with common issues and solutions
- Updated file structure documentation
- Added quick commands reference for easy access
- Improved monitoring and health check instructions
- Added next steps section for deployment completion
</commit_message>
<xml_diff>
--- a/webpages.xlsx
+++ b/webpages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericyang/git/webtracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016079C5-04F7-794B-AD55-939FB68DA50F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7F2ADD-E184-EA4F-9F58-70430C6C7A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37480" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Webpages" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>URL</t>
   </si>
@@ -80,13 +80,91 @@
   </si>
   <si>
     <t>https://www.cmcmarkets.com/preview/zh-au/cfd/fx-active</t>
+  </si>
+  <si>
+    <t>https://www.cmcmarkets.com/preview/en-nz/cfd</t>
+  </si>
+  <si>
+    <t>https://www.cmcmarkets.com/preview/en-nz/cfd/fx-active</t>
+  </si>
+  <si>
+    <t>https://www.cmcmarkets.com/preview/en-nz/cfd/pricing</t>
+  </si>
+  <si>
+    <t>https://www.cmcmarkets.com/preview/en-nz/cfd/products/forex</t>
+  </si>
+  <si>
+    <t>https://www.cmcmarkets.com/preview/en-nz/cfd/products/indices</t>
+  </si>
+  <si>
+    <t>https://www.cmcmarkets.com/preview/en-nz/cfd/products/commodities</t>
+  </si>
+  <si>
+    <t>https://www.cmcmarkets.com/preview/en-nz/cfd/products/shares</t>
+  </si>
+  <si>
+    <t>https://www.cmcmarkets.com/preview/en-nz/cfd/products/cryptocurrencies</t>
+  </si>
+  <si>
+    <t>https://www.cmcmarkets.com/preview/en-nz/cfd/products/etf-trading</t>
+  </si>
+  <si>
+    <t>https://www.cmcmarkets.com/preview/en-nz/legal-documents</t>
+  </si>
+  <si>
+    <t>https://www.cmcmarkets.com/preview/en-nz/legal-documents/cfd-legal-documents</t>
+  </si>
+  <si>
+    <t>https://www.cmcmarkets.com/preview/en-nz/legal-documents/mt4-legal-documents</t>
+  </si>
+  <si>
+    <t>https://www.cmcmarkets.com/preview/en-nz/legal-documents/other-legal-documents</t>
+  </si>
+  <si>
+    <t>https://www.cmcmarkets.com/preview/zh-nz/cfd</t>
+  </si>
+  <si>
+    <t>https://www.cmcmarkets.com/preview/zh-nz/cfd/fx-active</t>
+  </si>
+  <si>
+    <t>https://www.cmcmarkets.com/preview/zh-nz/cfd/pricing</t>
+  </si>
+  <si>
+    <t>https://www.cmcmarkets.com/preview/zh-nz/cfd/products/forex</t>
+  </si>
+  <si>
+    <t>https://www.cmcmarkets.com/preview/zh-nz/cfd/products/indices</t>
+  </si>
+  <si>
+    <t>https://www.cmcmarkets.com/preview/zh-nz/cfd/products/commodities</t>
+  </si>
+  <si>
+    <t>https://www.cmcmarkets.com/preview/zh-nz/cfd/products/shares</t>
+  </si>
+  <si>
+    <t>https://www.cmcmarkets.com/preview/zh-nz/cfd/products/cryptocurrencies</t>
+  </si>
+  <si>
+    <t>https://www.cmcmarkets.com/preview/zh-nz/cfd/products/etf-trading</t>
+  </si>
+  <si>
+    <t>https://www.cmcmarkets.com/preview/zh-nz/legal-documents</t>
+  </si>
+  <si>
+    <t>https://www.cmcmarkets.com/preview/zh-nz/legal-documents/cfd-legal-documents</t>
+  </si>
+  <si>
+    <t>http://cmcmarkets.com/preview/zh-nz/legal-documents/mt4-legal-documents</t>
+  </si>
+  <si>
+    <t>https://www.cmcmarkets.com/preview/zh-nz/legal-documents/other-legal-documents</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +179,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -124,9 +208,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -430,15 +515,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A38" activeCellId="1" sqref="A31:XFD31 A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.5" customWidth="1"/>
+    <col min="1" max="1" width="75" customWidth="1"/>
     <col min="2" max="2" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -516,6 +601,136 @@
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement new Excel-based structure with en/zh folders and remove translation functionality
</commit_message>
<xml_diff>
--- a/webpages.xlsx
+++ b/webpages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericyang/git/webtracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7F2ADD-E184-EA4F-9F58-70430C6C7A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA07F21-7D7D-D942-9616-27E7D2C35B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37480" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Webpages" sheetId="1" r:id="rId1"/>
@@ -515,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A38" activeCellId="1" sqref="A31:XFD31 A38"/>
+      <selection activeCell="H12" sqref="H12:H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -527,7 +527,7 @@
     <col min="2" max="2" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -538,7 +538,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -549,7 +549,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -560,7 +560,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -571,7 +571,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -582,7 +582,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -593,143 +593,143 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H12" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H13" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H14" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H15" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H16" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H17" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="19" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H19" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="20" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="21" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="22" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="23" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H23" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="24" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H24" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="25" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H25" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="26" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H26" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="27" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H27" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="28" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H28" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="29" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H29" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="30" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H30" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="31" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H31" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="32" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H32" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="33" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H33" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="34" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H34" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>